<commit_message>
adding another excel file
</commit_message>
<xml_diff>
--- a/amazon/src/test/testData/TestData.xlsx
+++ b/amazon/src/test/testData/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Afnan\Desktop\New_Amazon\amazon\amazon\src\test\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Afnan\Desktop\Group_Project\amazon\src\test\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533C92EA-97AE-4AB0-9B3A-8482771D4BF0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4941155-2972-426E-9C23-247613A439D1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8730" xr2:uid="{0CD4F209-AE29-4DE4-857F-E366E988CACC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>email</t>
   </si>
@@ -33,29 +33,100 @@
     <t>password</t>
   </si>
   <si>
-    <t>ads@hotmail.com</t>
-  </si>
-  <si>
-    <t>ghj@hotmail.com</t>
-  </si>
-  <si>
-    <t>dgh@yahoo.com</t>
-  </si>
-  <si>
-    <t>dfghj</t>
-  </si>
-  <si>
-    <t>ghjk</t>
+    <t>acdf@hotmail.com</t>
+  </si>
+  <si>
+    <t>acd2f@hotmail.com</t>
+  </si>
+  <si>
+    <t>xcvb4567</t>
+  </si>
+  <si>
+    <t>acdf3@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf4@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf5@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf6@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf7@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf8@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf9@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf10@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf11@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf12@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf13@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf14@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf15@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf16@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf17@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf18@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf19@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf20@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf21@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf22@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf23@hotmail.com</t>
+  </si>
+  <si>
+    <t>acdf24@hotmail.com</t>
+  </si>
+  <si>
+    <t>ncwchewcdc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,13 +149,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C81396-7928-4192-88BC-159F2E20D015}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B24" activeCellId="11" sqref="B2 B4 B6 B8 B10 B12 B14 B16 B18 B20 B22 B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -417,30 +496,224 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{D1D2D16E-FC62-445B-9E9E-6F254E27E038}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{638CEA95-A47D-4E7F-BA7F-0864B6A4E7E2}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{E0B10CB2-1743-49A5-84B6-1878B1288B2A}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{5ADFDB0E-96B7-4616-8A7C-BA1EF03C71A7}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{F8E42303-374B-416A-8D30-1688A4B1E1B1}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{9DF702F4-2420-480A-AE2B-2CB802BF80DE}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{5CF076AA-5F34-48DD-81A7-EB4530F73DFC}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{92AD4FD5-EE15-4390-9548-E34D2221523C}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{34A35DB1-D513-40D3-8C99-BA359EA9A1C9}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{32F48F1E-91B1-419C-95A8-B929B6598DB2}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{9EF3B602-B3A0-429E-A211-649F9684D30C}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{6B87E5B1-C122-4540-8908-0918FB2629A9}"/>
+    <hyperlink ref="A14" r:id="rId13" xr:uid="{0BE1379C-BECD-41D5-AC05-B1CC01A900C5}"/>
+    <hyperlink ref="A15" r:id="rId14" xr:uid="{A5C8D09C-45B3-43D0-BB04-B31A6A131186}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{E6C7BCDD-53FA-4924-A36E-1B0C8A27312E}"/>
+    <hyperlink ref="A17" r:id="rId16" xr:uid="{81F07088-0250-4FDA-A767-8A5BB98E8034}"/>
+    <hyperlink ref="A18" r:id="rId17" xr:uid="{CE4EAD6F-E3CD-45E6-B0B5-A798CC22D3FC}"/>
+    <hyperlink ref="A19" r:id="rId18" xr:uid="{BF720D8C-8183-4631-8F9D-09DACB47E284}"/>
+    <hyperlink ref="A20" r:id="rId19" xr:uid="{AF0BE939-9DBE-472D-B2CE-26A480EB9201}"/>
+    <hyperlink ref="A21" r:id="rId20" xr:uid="{152B6255-7E55-40DE-9202-34AEBCD0E6D7}"/>
+    <hyperlink ref="A22" r:id="rId21" xr:uid="{1654C8A5-F8EF-46F0-9BB8-EA418088AEC1}"/>
+    <hyperlink ref="A23" r:id="rId22" xr:uid="{5A904C2D-D5BA-4476-A4B0-E9727D55F412}"/>
+    <hyperlink ref="A24" r:id="rId23" xr:uid="{6E83EB2F-FFA9-420E-BF65-2C0D52542127}"/>
+    <hyperlink ref="A25" r:id="rId24" xr:uid="{3CC70A20-500D-45CC-92FD-3ECEF752E820}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>